<commit_message>
adding new excel file read
</commit_message>
<xml_diff>
--- a/APIFLab/src/test/resources/ExelData/Book1 - Copy.xlsx
+++ b/APIFLab/src/test/resources/ExelData/Book1 - Copy.xlsx
@@ -1,22 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23328"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{F16F4FF1-A634-40F4-AD00-7EE193CA8D65}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="108" windowWidth="16212" windowHeight="5808"/>
+    <workbookView xWindow="1425" yWindow="1425" windowWidth="16245" windowHeight="9210" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="newpage1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="0"/>
+  <oleSize ref="A1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="13">
   <si>
     <t>user Name</t>
   </si>
@@ -60,8 +62,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -111,6 +113,14 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -157,7 +167,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -189,9 +199,27 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -223,6 +251,24 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -398,22 +444,22 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+      <selection activeCell="C2" sqref="C2:C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.109375" customWidth="1"/>
-    <col min="2" max="2" width="10.5546875" customWidth="1"/>
+    <col min="1" max="1" width="15.140625" customWidth="1"/>
+    <col min="2" max="2" width="10.5703125" customWidth="1"/>
     <col min="3" max="3" width="21" customWidth="1"/>
-    <col min="4" max="4" width="20.33203125" customWidth="1"/>
+    <col min="4" max="4" width="20.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -430,7 +476,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -444,19 +490,21 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:6">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>7</v>
       </c>
       <c r="B3">
         <v>8678576</v>
       </c>
-      <c r="C3" s="1"/>
+      <c r="C3" s="1" t="s">
+        <v>5</v>
+      </c>
       <c r="D3" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:6">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>8</v>
       </c>
@@ -469,22 +517,23 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C2" r:id="rId1"/>
-    <hyperlink ref="C4" r:id="rId2"/>
+    <hyperlink ref="C2" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="C4" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="C3" r:id="rId3" xr:uid="{384FD95B-6137-4D71-8601-0816E53CB752}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:1">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>9</v>
       </c>
@@ -495,12 +544,12 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>